<commit_message>
Updating MW Unit 1.2 exercises
</commit_message>
<xml_diff>
--- a/01-Class-Activities/Mon-Wed-Class/01-Excel/2/Activities/01-Ins_ExcelPlayground/Solved/Excel_Playground_Starter.xlsx
+++ b/01-Class-Activities/Mon-Wed-Class/01-Excel/2/Activities/01-Ins_ExcelPlayground/Solved/Excel_Playground_Starter.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afhaque/TrilogyWork/DataViz-Lesson-Plans/01-Lesson-Plans/01-Excel/2/Activities/01-Ins_ExcelPlayground/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\98452\Documents\GitHub\GWU-ARL-DATA-PT-09-2019-U-C\01-Class-Activities\Mon-Wed-Class\01-Excel\2\Activities\01-Ins_ExcelPlayground\Solved\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14565" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -44,9 +44,6 @@
     <t>Grade 3</t>
   </si>
   <si>
-    <t>Reynold Anderson</t>
-  </si>
-  <si>
     <t>Average Score</t>
   </si>
   <si>
@@ -56,30 +53,6 @@
     <t>Final Score</t>
   </si>
   <si>
-    <t>Carlton Hashim</t>
-  </si>
-  <si>
-    <t>Veríssimo Carl</t>
-  </si>
-  <si>
-    <t>Kip Zayn</t>
-  </si>
-  <si>
-    <t>Rupert Mateus</t>
-  </si>
-  <si>
-    <t>Mason Toby</t>
-  </si>
-  <si>
-    <t>Randell Dominicus</t>
-  </si>
-  <si>
-    <t>Violet Hovsep</t>
-  </si>
-  <si>
-    <t>Evangeline Elisavet</t>
-  </si>
-  <si>
     <t>Summary</t>
   </si>
   <si>
@@ -96,12 +69,39 @@
   </si>
   <si>
     <t>Std. Deviation</t>
+  </si>
+  <si>
+    <t>John Culhane</t>
+  </si>
+  <si>
+    <t>Aaron Isaacson</t>
+  </si>
+  <si>
+    <t>Alex Black</t>
+  </si>
+  <si>
+    <t>Chandra Kent</t>
+  </si>
+  <si>
+    <t>Hythem Khalil</t>
+  </si>
+  <si>
+    <t>Mario Iglesias</t>
+  </si>
+  <si>
+    <t>Jack Woltman</t>
+  </si>
+  <si>
+    <t>Julian Tosani</t>
+  </si>
+  <si>
+    <t>Thomas Burless</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -192,11 +192,42 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -467,23 +498,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.125" customWidth="1"/>
+    <col min="4" max="4" width="13.125" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -500,22 +529,22 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>89</v>
@@ -532,12 +561,12 @@
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>92</v>
@@ -554,12 +583,12 @@
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>86</v>
@@ -576,12 +605,12 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>82</v>
@@ -598,12 +627,12 @@
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>94</v>
@@ -620,12 +649,12 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>95</v>
@@ -642,12 +671,12 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>86</v>
@@ -664,12 +693,12 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>85</v>
@@ -686,12 +715,12 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>100</v>
@@ -708,44 +737,44 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B19" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding class activities for Saturday
</commit_message>
<xml_diff>
--- a/01-Class-Activities/Mon-Wed-Class/01-Excel/2/Activities/01-Ins_ExcelPlayground/Solved/Excel_Playground_Starter.xlsx
+++ b/01-Class-Activities/Mon-Wed-Class/01-Excel/2/Activities/01-Ins_ExcelPlayground/Solved/Excel_Playground_Starter.xlsx
@@ -550,16 +550,22 @@
         <v>89</v>
       </c>
       <c r="D2">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="E2">
         <v>92</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="3">
+        <f>AVERAGE(C2:E2)</f>
+        <v>69.666666666666671</v>
+      </c>
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" s="3"/>
+      <c r="H2" s="3">
+        <f>SUM(F2,G2)</f>
+        <v>70.666666666666671</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -577,11 +583,17 @@
       <c r="E3">
         <v>97</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3">
+        <f>AVERAGE(C3:E3)</f>
+        <v>94</v>
+      </c>
       <c r="G3">
         <v>3</v>
       </c>
-      <c r="H3" s="3"/>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H10" si="0">SUM(F3,G3)</f>
+        <v>97</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -599,11 +611,17 @@
       <c r="E4">
         <v>84</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3">
+        <f t="shared" ref="F4:F10" si="1">AVERAGE(C4:E4)</f>
+        <v>89.333333333333329</v>
+      </c>
       <c r="G4">
         <v>4</v>
       </c>
-      <c r="H4" s="3"/>
+      <c r="H4" s="3">
+        <f t="shared" si="0"/>
+        <v>93.333333333333329</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -621,11 +639,17 @@
       <c r="E5">
         <v>97</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="3">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -641,13 +665,19 @@
         <v>87</v>
       </c>
       <c r="E6">
-        <v>83</v>
-      </c>
-      <c r="F6" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="1"/>
+        <v>61.333333333333336</v>
+      </c>
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6" s="3"/>
+      <c r="H6" s="3">
+        <f t="shared" si="0"/>
+        <v>62.333333333333336</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -665,11 +695,17 @@
       <c r="E7">
         <v>97</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3">
+        <f t="shared" si="1"/>
+        <v>94.666666666666671</v>
+      </c>
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="H7" s="3"/>
+      <c r="H7" s="3">
+        <f t="shared" si="0"/>
+        <v>95.666666666666671</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -687,11 +723,17 @@
       <c r="E8">
         <v>93</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3">
+        <f t="shared" si="1"/>
+        <v>90.666666666666671</v>
+      </c>
       <c r="G8">
         <v>2</v>
       </c>
-      <c r="H8" s="3"/>
+      <c r="H8" s="3">
+        <f t="shared" si="0"/>
+        <v>92.666666666666671</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -709,11 +751,17 @@
       <c r="E9">
         <v>97</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3">
+        <f t="shared" si="1"/>
+        <v>89.333333333333329</v>
+      </c>
       <c r="G9">
         <v>3</v>
       </c>
-      <c r="H9" s="3"/>
+      <c r="H9" s="3">
+        <f t="shared" si="0"/>
+        <v>92.333333333333329</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -731,11 +779,17 @@
       <c r="E10">
         <v>96</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3">
+        <f t="shared" si="1"/>
+        <v>93.666666666666671</v>
+      </c>
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10" s="3"/>
+      <c r="H10" s="3">
+        <f t="shared" si="0"/>
+        <v>93.666666666666671</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -747,31 +801,46 @@
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="6">
+        <f>AVERAGE(H2:H10)</f>
+        <v>87.296296296296291</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="6">
+        <f>MEDIAN(H2:H10)</f>
+        <v>92.666666666666671</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="6">
+        <f>MAX(H2:H10)</f>
+        <v>97</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="6">
+        <f>MIN(H2:H10)</f>
+        <v>62.333333333333336</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="5">
+        <f>STDEV(H1:H10)</f>
+        <v>12.225252149688234</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>